<commit_message>
Rewired for more consistent power delivery across mechanisms (2105A.c, 2105A motors.xlsx) Edited lift function for left/right designations instead of A-F Added deadbanding for 2105A-john.h
</commit_message>
<xml_diff>
--- a/docs/2105A motors.xlsx
+++ b/docs/2105A motors.xlsx
@@ -421,7 +421,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,10 +454,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -468,7 +468,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
         <v>10</v>
@@ -482,10 +482,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -552,10 +552,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -566,7 +566,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
@@ -580,10 +580,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated 2105A motor configuration Uploaded basic 2105B code (driver only, all in 1 C file)
</commit_message>
<xml_diff>
--- a/docs/2105A motors.xlsx
+++ b/docs/2105A motors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="45" windowWidth="21075" windowHeight="10035"/>
+    <workbookView xWindow="240" yWindow="45" windowWidth="20730" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
   <si>
     <t>Port</t>
   </si>
@@ -71,6 +71,12 @@
   </si>
   <si>
     <t>LiftRightC</t>
+  </si>
+  <si>
+    <t>NewPE</t>
+  </si>
+  <si>
+    <t>NewMotor</t>
   </si>
 </sst>
 </file>
@@ -94,12 +100,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -114,9 +126,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,9 +443,11 @@
     <col min="2" max="2" width="4.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -445,8 +460,14 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -459,8 +480,14 @@
       <c r="D2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -473,8 +500,14 @@
       <c r="D3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -487,8 +520,14 @@
       <c r="D4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -501,8 +540,14 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -515,8 +560,14 @@
       <c r="D6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -529,8 +580,14 @@
       <c r="D7" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -543,8 +600,14 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -557,8 +620,14 @@
       <c r="D9" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -571,8 +640,14 @@
       <c r="D10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -584,6 +659,12 @@
       </c>
       <c r="D11" t="s">
         <v>18</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved drive motors to cortex
</commit_message>
<xml_diff>
--- a/docs/2105A motors.xlsx
+++ b/docs/2105A motors.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="22">
   <si>
     <t>Port</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>NewMotor</t>
+  </si>
+  <si>
+    <t>New2PE</t>
   </si>
 </sst>
 </file>
@@ -431,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,7 +450,7 @@
     <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -466,8 +469,11 @@
       <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -486,8 +492,11 @@
       <c r="F2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -506,8 +515,11 @@
       <c r="F3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -526,8 +538,11 @@
       <c r="F4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -546,8 +561,11 @@
       <c r="F5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -566,8 +584,11 @@
       <c r="F6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -586,8 +607,11 @@
       <c r="F7" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -606,8 +630,11 @@
       <c r="F8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -626,8 +653,11 @@
       <c r="F9" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -646,8 +676,11 @@
       <c r="F10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -664,6 +697,9 @@
         <v>18</v>
       </c>
       <c r="F11" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>